<commit_message>
Change price to float
</commit_message>
<xml_diff>
--- a/build_dashboard_dataset/pricediffavg.xlsx
+++ b/build_dashboard_dataset/pricediffavg.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>datasource</t>
   </si>
@@ -26,12 +26,6 @@
   </si>
   <si>
     <t>Target Deals Website</t>
-  </si>
-  <si>
-    <t>118.86178</t>
-  </si>
-  <si>
-    <t>136.39731</t>
   </si>
 </sst>
 </file>
@@ -407,16 +401,16 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
+      <c r="B2">
+        <v>118.86178</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
+      <c r="B3">
+        <v>136.39731</v>
       </c>
     </row>
   </sheetData>

</xml_diff>